<commit_message>
EPBDS-9060 method doesn't work for spreadsheet cell range with empty cells
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7003.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7003.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0C23F3-AB22-45B1-BADF-0D9C32BA2429}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>X1</t>
   </si>
@@ -75,12 +84,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,13 +103,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442" rgb="1F497D"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -196,36 +204,36 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -242,10 +250,10 @@
   <a:themeElements>
     <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -280,7 +288,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -332,7 +340,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -437,7 +445,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -446,13 +454,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -462,7 +470,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -471,7 +479,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -480,7 +488,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -490,12 +498,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -526,7 +534,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -545,7 +553,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -557,19 +565,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="46.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="49.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" width="46.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -615,7 +623,9 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
@@ -674,7 +684,9 @@
       <c r="C13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="E13" s="11" t="s">
         <v>14</v>
       </c>
@@ -684,30 +696,30 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B10:E10"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-12532 Spreadsheet step type should be identified from Excel cell type if step type is not provided
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7003.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7003.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0C23F3-AB22-45B1-BADF-0D9C32BA2429}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75A8AB9-C898-FE44-A180-99EBAF0FFD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>X1</t>
   </si>
@@ -79,6 +83,33 @@
   </si>
   <si>
     <t>_res_.$X2$Y4</t>
+  </si>
+  <si>
+    <t>Y5</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>_res_.$X2$Y5</t>
+  </si>
+  <si>
+    <t>Y6</t>
+  </si>
+  <si>
+    <t>Y7</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>_res_.$X2$Y6</t>
+  </si>
+  <si>
+    <t>_res_.$X2$Y7</t>
   </si>
 </sst>
 </file>
@@ -206,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -219,6 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -228,9 +260,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -246,9 +285,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -286,7 +325,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -392,7 +431,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -566,28 +605,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:K13"/>
+  <dimension ref="B3:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="46.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
         <v>0</v>
@@ -596,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -608,7 +648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -619,7 +659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -630,71 +670,134 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="18">
+        <v>34284</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="F15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="F16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>14</v>
+      <c r="G17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -706,7 +809,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -718,7 +821,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>